<commit_message>
testing small data is work
</commit_message>
<xml_diff>
--- a/public/myanmar name.xlsx
+++ b/public/myanmar name.xlsx
@@ -409,22 +409,17 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>လင်းလင်း</v>
+        <v>မန်ကျီးပင်</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>မောင်မောင်</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>မြမောင်</v>
+        <v>ရေကျော်</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>ဦးလှ</v>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>